<commit_message>
Streamlitform_2 : Working form code
</commit_message>
<xml_diff>
--- a/data_set.xlsx
+++ b/data_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathu\OneDrive\Documents\Ideathon\Ideathon_Streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737FE0D5-881C-49E5-BF47-6452E78A4AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CE0A24-95D2-4E99-AAA6-8FD28AFA6A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="100">
   <si>
     <t>Line Num.</t>
   </si>
@@ -682,9 +682,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="P43" sqref="A24:P43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1431,7 +1433,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1475,7 +1477,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1519,7 +1521,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1563,7 +1565,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1607,7 +1609,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1651,7 +1653,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1689,7 +1691,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1734,526 +1736,6 @@
       </c>
       <c r="O23" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="O24" t="s">
-        <v>68</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="O25" t="s">
-        <v>78</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="O26" t="s">
-        <v>78</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="O27" t="s">
-        <v>78</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="O28" t="s">
-        <v>78</v>
-      </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="O29" t="s">
-        <v>78</v>
-      </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="O30" t="s">
-        <v>78</v>
-      </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="O31" t="s">
-        <v>78</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="O32" t="s">
-        <v>78</v>
-      </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="O33" t="s">
-        <v>78</v>
-      </c>
-      <c r="P33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="O34" t="s">
-        <v>78</v>
-      </c>
-      <c r="P34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="O35" t="s">
-        <v>78</v>
-      </c>
-      <c r="P35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-      <c r="O36" t="s">
-        <v>78</v>
-      </c>
-      <c r="P36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="O37" t="s">
-        <v>78</v>
-      </c>
-      <c r="P37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="O38" t="s">
-        <v>78</v>
-      </c>
-      <c r="P38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="O39" t="s">
-        <v>78</v>
-      </c>
-      <c r="P39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="O40" t="s">
-        <v>78</v>
-      </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="O41" t="s">
-        <v>78</v>
-      </c>
-      <c r="P41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="O42" t="s">
-        <v>29</v>
-      </c>
-      <c r="P42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="O43" t="s">
-        <v>29</v>
-      </c>
-      <c r="P43">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More changes made to the data_set
</commit_message>
<xml_diff>
--- a/data_set.xlsx
+++ b/data_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathu\OneDrive\Documents\Ideathon\Ideathon_Streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EBF14B-A740-4A21-8645-457F849ED4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAA12ED-B785-4501-9430-2942EBB01161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="109">
   <si>
     <t>Line Num.</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Subsystem</t>
   </si>
   <si>
-    <t>MaterialCost</t>
-  </si>
-  <si>
     <t>Engine</t>
   </si>
   <si>
@@ -354,6 +351,15 @@
   </si>
   <si>
     <t>LCO 3.8V</t>
+  </si>
+  <si>
+    <t>Battery Management System</t>
+  </si>
+  <si>
+    <t>Orion BMS 2</t>
+  </si>
+  <si>
+    <t>Critical Component</t>
   </si>
 </sst>
 </file>
@@ -716,21 +722,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="37.42578125" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -776,25 +783,22 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
       </c>
       <c r="F2">
         <v>621</v>
@@ -819,30 +823,30 @@
         <v>1569</v>
       </c>
       <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
       </c>
       <c r="F3">
         <v>581</v>
@@ -867,30 +871,30 @@
         <v>622.5</v>
       </c>
       <c r="M3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
       </c>
       <c r="F4">
         <v>151</v>
@@ -915,27 +919,27 @@
         <v>1866</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
       </c>
       <c r="F5">
         <v>268</v>
@@ -960,30 +964,30 @@
         <v>1133</v>
       </c>
       <c r="M5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
       </c>
       <c r="F6">
         <v>125</v>
@@ -1008,30 +1012,30 @@
         <v>888</v>
       </c>
       <c r="M6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>41</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -1056,30 +1060,30 @@
         <v>359</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N7">
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>44</v>
-      </c>
-      <c r="E8" t="s">
-        <v>45</v>
       </c>
       <c r="F8">
         <v>130</v>
@@ -1104,30 +1108,30 @@
         <v>373</v>
       </c>
       <c r="M8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>48</v>
-      </c>
-      <c r="E9" t="s">
-        <v>49</v>
       </c>
       <c r="F9">
         <v>150</v>
@@ -1152,30 +1156,30 @@
         <v>969</v>
       </c>
       <c r="M9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
         <v>51</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" t="s">
-        <v>53</v>
       </c>
       <c r="F10">
         <v>166</v>
@@ -1200,30 +1204,30 @@
         <v>2091</v>
       </c>
       <c r="M10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N10">
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
         <v>55</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>56</v>
-      </c>
-      <c r="E11" t="s">
-        <v>57</v>
       </c>
       <c r="F11">
         <v>80</v>
@@ -1248,30 +1252,30 @@
         <v>664.5</v>
       </c>
       <c r="M11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N11">
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
         <v>59</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>61</v>
-      </c>
-      <c r="E12" t="s">
-        <v>62</v>
       </c>
       <c r="F12">
         <v>58</v>
@@ -1296,30 +1300,30 @@
         <v>346</v>
       </c>
       <c r="M12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N12">
         <v>1</v>
       </c>
       <c r="O12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
         <v>64</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>65</v>
-      </c>
-      <c r="E13" t="s">
-        <v>66</v>
       </c>
       <c r="F13">
         <v>60</v>
@@ -1344,27 +1348,27 @@
         <v>619</v>
       </c>
       <c r="M13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>69</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>71</v>
       </c>
       <c r="F14">
         <v>4500</v>
@@ -1389,27 +1393,27 @@
         <v>4991</v>
       </c>
       <c r="M14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
         <v>73</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>74</v>
-      </c>
-      <c r="E15" t="s">
-        <v>75</v>
       </c>
       <c r="F15">
         <v>8</v>
@@ -1434,27 +1438,27 @@
         <v>683</v>
       </c>
       <c r="M15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
         <v>76</v>
-      </c>
-      <c r="D16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" t="s">
-        <v>77</v>
       </c>
       <c r="F16">
         <v>59</v>
@@ -1479,10 +1483,10 @@
         <v>4508</v>
       </c>
       <c r="M16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1490,16 +1494,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
         <v>78</v>
       </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>79</v>
-      </c>
-      <c r="E17" t="s">
-        <v>80</v>
       </c>
       <c r="F17">
         <v>51</v>
@@ -1524,10 +1528,10 @@
         <v>837</v>
       </c>
       <c r="M17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1535,16 +1539,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" t="s">
         <v>82</v>
-      </c>
-      <c r="E18" t="s">
-        <v>83</v>
       </c>
       <c r="F18">
         <v>34</v>
@@ -1569,10 +1573,10 @@
         <v>1184</v>
       </c>
       <c r="M18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1580,16 +1584,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
         <v>84</v>
-      </c>
-      <c r="E19" t="s">
-        <v>85</v>
       </c>
       <c r="F19">
         <v>33</v>
@@ -1614,10 +1618,10 @@
         <v>1707</v>
       </c>
       <c r="M19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1625,16 +1629,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s">
         <v>87</v>
-      </c>
-      <c r="E20" t="s">
-        <v>88</v>
       </c>
       <c r="F20">
         <v>50</v>
@@ -1659,10 +1663,10 @@
         <v>1279</v>
       </c>
       <c r="M20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1670,16 +1674,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
         <v>89</v>
       </c>
-      <c r="C21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>90</v>
-      </c>
-      <c r="E21" t="s">
-        <v>91</v>
       </c>
       <c r="F21">
         <v>600</v>
@@ -1704,10 +1708,10 @@
         <v>2672</v>
       </c>
       <c r="M21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1715,16 +1719,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" t="s">
         <v>100</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>101</v>
-      </c>
-      <c r="E22" t="s">
-        <v>102</v>
       </c>
       <c r="F22">
         <v>300</v>
@@ -1748,22 +1752,28 @@
         <f t="shared" si="1"/>
         <v>2550</v>
       </c>
+      <c r="M22" t="s">
+        <v>36</v>
+      </c>
+      <c r="O22" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" t="s">
         <v>103</v>
-      </c>
-      <c r="E23" t="s">
-        <v>104</v>
       </c>
       <c r="F23">
         <v>40</v>
@@ -1787,8 +1797,11 @@
         <f t="shared" si="1"/>
         <v>915</v>
       </c>
+      <c r="M23" t="s">
+        <v>36</v>
+      </c>
       <c r="O23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1796,16 +1809,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" t="s">
         <v>105</v>
-      </c>
-      <c r="E24" t="s">
-        <v>106</v>
       </c>
       <c r="F24">
         <v>35</v>
@@ -1829,22 +1842,28 @@
         <f t="shared" si="1"/>
         <v>3540</v>
       </c>
+      <c r="M24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O24" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" t="s">
         <v>92</v>
-      </c>
-      <c r="E25" t="s">
-        <v>93</v>
       </c>
       <c r="F25">
         <v>40</v>
@@ -1863,10 +1882,10 @@
         <v>522</v>
       </c>
       <c r="M25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1874,47 +1893,92 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="F26">
-        <v>100</v>
+        <v>1230</v>
       </c>
       <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
         <v>30</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
       </c>
       <c r="I26">
         <v>30</v>
       </c>
       <c r="J26">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="L26">
         <f t="shared" si="1"/>
+        <v>2630</v>
+      </c>
+      <c r="M26" t="s">
+        <v>108</v>
+      </c>
+      <c r="O26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+      <c r="G27">
+        <v>30</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>30</v>
+      </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <f>F27*G27+H27+I27+J27+K27</f>
         <v>3037</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M27" t="s">
+        <v>97</v>
+      </c>
+      <c r="N27" t="s">
         <v>98</v>
       </c>
-      <c r="N26" t="s">
-        <v>99</v>
-      </c>
-      <c r="O26" t="s">
-        <v>95</v>
+      <c r="O27" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>